<commit_message>
Lisää paikkauskohteen Nro pakolliseksi merkityksi exceliin
</commit_message>
<xml_diff>
--- a/resources/public/excel/harja_paikkauskohteet_pohja.xlsx
+++ b/resources/public/excel/harja_paikkauskohteet_pohja.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markusva/repos/harja/resources/public/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markusva/repos/GitHub/harja/resources/public/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{406A2B0B-2C99-D948-B4B2-DF08757FED7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0758D801-0C88-E142-8B70-FB84BE4888F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33000" windowHeight="14400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="14400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Paikkausmallipohja" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>Työmenetelmä ja yksikkö: käytä valikon valmiita valintoja</t>
   </si>
   <si>
-    <t>Nro</t>
-  </si>
-  <si>
     <t>Kohteen nimi *</t>
   </si>
   <si>
@@ -200,6 +197,9 @@
   </si>
   <si>
     <t>Muu päällysteiden paikkaustyö</t>
+  </si>
+  <si>
+    <t>Nro *</t>
   </si>
 </sst>
 </file>
@@ -417,51 +417,46 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -487,7 +482,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -512,14 +507,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
@@ -541,16 +533,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -566,7 +555,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -588,7 +577,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -598,12 +586,15 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Hyperlinkki" xfId="2" builtinId="8"/>
+    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
     <cellStyle name="Normaali 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pilkku" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -687,7 +678,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -986,439 +977,433 @@
   <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="2"/>
-    <col min="2" max="2" width="37" style="3" customWidth="1"/>
-    <col min="3" max="8" width="8.83203125" style="3"/>
-    <col min="9" max="10" width="12.83203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="50.83203125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="16.83203125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" style="3"/>
-    <col min="14" max="14" width="16.83203125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="50.83203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="37" customWidth="1"/>
+    <col min="9" max="10" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="50.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="16.83203125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="50.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="10"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="10"/>
+      <c r="A2" s="62"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="8"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="13" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="10"/>
-    </row>
-    <row r="4" spans="1:15" s="25" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A4" s="16" t="s">
+      <c r="L3"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="8"/>
+    </row>
+    <row r="4" spans="1:15" s="22" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+      <c r="A4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="C4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="D4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="E4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="F4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="G4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="H4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="I4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="J4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="K4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="L4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="M4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="N4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="23" t="s">
+      <c r="O4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="24" t="s">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="60"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A6" s="23"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="60"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A7" s="23"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="60"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A8" s="23"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="60"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A9" s="23"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="60"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A10" s="23"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="36"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="60"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A11" s="23"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="60"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A12" s="23"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="60"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A13" s="23"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="60"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A14" s="23"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="60"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A15" s="23"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="60"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A16" s="23"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="60"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A17" s="23"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="60"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A18" s="23"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="30"/>
+      <c r="O18" s="60"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A19" s="23"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="41"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="60"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A20" s="23"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="30"/>
+      <c r="O20" s="60"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A21" s="42"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="49"/>
+      <c r="O21" s="61"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A22" s="50" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A5" s="26"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="66"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A6" s="26"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="66"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A7" s="26"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
-      <c r="I7" s="29"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="66"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A8" s="26"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="66"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A9" s="26"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="66"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A10" s="26"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="66"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A11" s="26"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="66"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A12" s="26"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="66"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A13" s="26"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="66"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A14" s="26"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="45"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="33"/>
-      <c r="O14" s="66"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A15" s="26"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="45"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="66"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A16" s="26"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="33"/>
-      <c r="O16" s="66"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A17" s="26"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="66"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A18" s="26"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="30"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="66"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A19" s="26"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="30"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="66"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A20" s="26"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="30"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="66"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A21" s="46"/>
-      <c r="B21" s="47"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="52"/>
-      <c r="M21" s="53"/>
-      <c r="N21" s="54"/>
-      <c r="O21" s="67"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A22" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="56"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="59"/>
-      <c r="L22" s="60"/>
-      <c r="M22" s="61"/>
-      <c r="N22" s="62">
+      <c r="B22" s="51"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="54"/>
+      <c r="L22" s="55"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="57">
         <f>SUM(N5:N21)</f>
         <v>0</v>
       </c>
-      <c r="O22" s="63"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="B25" s="64"/>
+      <c r="O22" s="58"/>
     </row>
     <row r="40" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="41" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1467,113 +1452,113 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="50.33203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="25" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="59" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="65" t="s">
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="59" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="65" t="s">
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="59" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" s="65" t="s">
+      <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="59" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" s="65" t="s">
+      <c r="B5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" s="59" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" s="65" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" s="59" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" s="65" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="59" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" s="65" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="59" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9" s="65" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" s="59" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10" s="65" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" s="59" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" s="65" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" s="59" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12" s="65" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" s="59" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13" s="65" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" s="59" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14" s="65" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" s="59" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15" s="65" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" s="59" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16" s="65" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17" s="59" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A17" s="65" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A18" s="59" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A18" s="65" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19" s="59" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A19" s="65" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uudet excelit muut paikkaukset ominaisuudelle.
Pohjaan lisätty * merkkaamaan pakollisesta numerosta. Excelin luontiin lisätty varoitus, ettei käyttäjä yritä muokata kohteita excelillä.
</commit_message>
<xml_diff>
--- a/resources/public/excel/harja_paikkauskohteet_pohja.xlsx
+++ b/resources/public/excel/harja_paikkauskohteet_pohja.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markusva/repos/harja/dev-resources/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markusva/repos/GitHub/harja/resources/public/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6376A06E-1C09-49D5-B4EF-C9692B3CE643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306171CE-180E-7C47-A586-5740B02E6C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33000" windowHeight="14400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="14400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Paikkausmallipohja" sheetId="1" r:id="rId1"/>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Työmenetelmä ja yksikkö: käytä valikon valmiita valintoja</t>
-  </si>
-  <si>
-    <t>Nro</t>
   </si>
   <si>
     <t>Kohteen nimi *</t>
@@ -203,6 +200,9 @@
   <si>
     <t>Muu päällysteiden paikkaustyö</t>
   </si>
+  <si>
+    <t>Nro *</t>
+  </si>
 </sst>
 </file>
 
@@ -213,7 +213,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* \-??\ _€_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="#,##0.00&quot; €&quot;"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -587,9 +587,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -617,6 +614,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -707,9 +707,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022 -teema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -747,7 +747,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -853,7 +853,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -995,7 +995,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1006,134 +1006,134 @@
   <dimension ref="A1:O237"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="37" customWidth="1"/>
-    <col min="9" max="10" width="12.875" customWidth="1"/>
-    <col min="11" max="11" width="50.875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="16.875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="50.875" style="3" customWidth="1"/>
+    <col min="9" max="10" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="50.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.83203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="16.83203125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="50.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="51" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
       <c r="K1" s="4"/>
       <c r="L1" s="5"/>
       <c r="M1" s="6"/>
       <c r="N1" s="7"/>
       <c r="O1" s="8"/>
     </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A2" s="61"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
       <c r="K2" s="4"/>
       <c r="L2" s="5"/>
       <c r="M2" s="6"/>
       <c r="N2" s="7"/>
       <c r="O2" s="8"/>
     </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="52" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A3" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="59">
+      <c r="B3" s="52"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="58">
         <f>SUM(N6:N236)</f>
         <v>0</v>
       </c>
-      <c r="O3" s="60"/>
-    </row>
-    <row r="4" spans="1:15" s="20" customFormat="1" ht="15">
+      <c r="O3" s="59"/>
+    </row>
+    <row r="4" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="61" t="s">
+      <c r="K4" s="60" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="23.25">
+    <row r="5" spans="1:15" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="D5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="E5" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="F5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="G5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="H5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="I5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="J5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="K5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="L5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="M5" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="17" t="s">
+      <c r="N5" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="N5" s="18" t="s">
+      <c r="O5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" s="21"/>
       <c r="B6" s="22"/>
       <c r="C6" s="23"/>
@@ -1150,7 +1150,7 @@
       <c r="N6" s="28"/>
       <c r="O6" s="50"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" s="21"/>
       <c r="B7" s="22"/>
       <c r="C7" s="29"/>
@@ -1167,7 +1167,7 @@
       <c r="N7" s="28"/>
       <c r="O7" s="50"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A8" s="21"/>
       <c r="B8" s="31"/>
       <c r="C8" s="29"/>
@@ -1184,7 +1184,7 @@
       <c r="N8" s="28"/>
       <c r="O8" s="50"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" s="21"/>
       <c r="B9" s="32"/>
       <c r="C9" s="23"/>
@@ -1201,7 +1201,7 @@
       <c r="N9" s="28"/>
       <c r="O9" s="50"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" s="21"/>
       <c r="B10" s="32"/>
       <c r="C10" s="29"/>
@@ -1218,7 +1218,7 @@
       <c r="N10" s="28"/>
       <c r="O10" s="50"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11" s="21"/>
       <c r="B11" s="32"/>
       <c r="C11" s="24"/>
@@ -1235,7 +1235,7 @@
       <c r="N11" s="28"/>
       <c r="O11" s="50"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12" s="21"/>
       <c r="B12" s="32"/>
       <c r="C12" s="23"/>
@@ -1252,7 +1252,7 @@
       <c r="N12" s="28"/>
       <c r="O12" s="50"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13" s="21"/>
       <c r="B13" s="35"/>
       <c r="C13" s="36"/>
@@ -1269,7 +1269,7 @@
       <c r="N13" s="28"/>
       <c r="O13" s="50"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14" s="21"/>
       <c r="B14" s="35"/>
       <c r="C14" s="36"/>
@@ -1286,7 +1286,7 @@
       <c r="N14" s="28"/>
       <c r="O14" s="50"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A15" s="21"/>
       <c r="B15" s="35"/>
       <c r="C15" s="36"/>
@@ -1303,7 +1303,7 @@
       <c r="N15" s="28"/>
       <c r="O15" s="50"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" s="21"/>
       <c r="B16" s="35"/>
       <c r="C16" s="36"/>
@@ -1320,7 +1320,7 @@
       <c r="N16" s="28"/>
       <c r="O16" s="50"/>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A17" s="21"/>
       <c r="B17" s="10"/>
       <c r="C17" s="23"/>
@@ -1337,7 +1337,7 @@
       <c r="N17" s="28"/>
       <c r="O17" s="50"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18" s="21"/>
       <c r="B18" s="32"/>
       <c r="C18" s="29"/>
@@ -1354,7 +1354,7 @@
       <c r="N18" s="28"/>
       <c r="O18" s="50"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A19" s="21"/>
       <c r="B19" s="32"/>
       <c r="C19" s="24"/>
@@ -1371,7 +1371,7 @@
       <c r="N19" s="28"/>
       <c r="O19" s="50"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20" s="21"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
@@ -1388,7 +1388,7 @@
       <c r="N20" s="28"/>
       <c r="O20" s="50"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A21" s="21"/>
       <c r="B21" s="35"/>
       <c r="C21" s="36"/>
@@ -1405,7 +1405,7 @@
       <c r="N21" s="28"/>
       <c r="O21" s="50"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A22" s="21"/>
       <c r="B22" s="35"/>
       <c r="C22" s="36"/>
@@ -1422,7 +1422,7 @@
       <c r="N22" s="28"/>
       <c r="O22" s="50"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A23" s="21"/>
       <c r="B23" s="35"/>
       <c r="C23" s="36"/>
@@ -1439,7 +1439,7 @@
       <c r="N23" s="28"/>
       <c r="O23" s="50"/>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A24" s="21"/>
       <c r="B24" s="35"/>
       <c r="C24" s="36"/>
@@ -1456,7 +1456,7 @@
       <c r="N24" s="28"/>
       <c r="O24" s="50"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A25" s="21"/>
       <c r="B25" s="35"/>
       <c r="C25" s="36"/>
@@ -1473,7 +1473,7 @@
       <c r="N25" s="28"/>
       <c r="O25" s="50"/>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A26" s="21"/>
       <c r="B26" s="35"/>
       <c r="C26" s="36"/>
@@ -1490,7 +1490,7 @@
       <c r="N26" s="28"/>
       <c r="O26" s="50"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A27" s="21"/>
       <c r="B27" s="35"/>
       <c r="C27" s="36"/>
@@ -1507,7 +1507,7 @@
       <c r="N27" s="28"/>
       <c r="O27" s="50"/>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A28" s="21"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
@@ -1524,7 +1524,7 @@
       <c r="N28" s="28"/>
       <c r="O28" s="50"/>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A29" s="21"/>
       <c r="B29" s="35"/>
       <c r="C29" s="36"/>
@@ -1541,7 +1541,7 @@
       <c r="N29" s="28"/>
       <c r="O29" s="50"/>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A30" s="21"/>
       <c r="B30" s="35"/>
       <c r="C30" s="36"/>
@@ -1558,7 +1558,7 @@
       <c r="N30" s="28"/>
       <c r="O30" s="50"/>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A31" s="21"/>
       <c r="B31" s="35"/>
       <c r="C31" s="36"/>
@@ -1575,7 +1575,7 @@
       <c r="N31" s="28"/>
       <c r="O31" s="50"/>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A32" s="21"/>
       <c r="B32" s="35"/>
       <c r="C32" s="36"/>
@@ -1592,7 +1592,7 @@
       <c r="N32" s="28"/>
       <c r="O32" s="50"/>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A33" s="21"/>
       <c r="B33" s="35"/>
       <c r="C33" s="36"/>
@@ -1609,7 +1609,7 @@
       <c r="N33" s="28"/>
       <c r="O33" s="50"/>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A34" s="21"/>
       <c r="B34" s="35"/>
       <c r="C34" s="36"/>
@@ -1626,7 +1626,7 @@
       <c r="N34" s="28"/>
       <c r="O34" s="50"/>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A35" s="21"/>
       <c r="B35" s="35"/>
       <c r="C35" s="36"/>
@@ -1643,7 +1643,7 @@
       <c r="N35" s="28"/>
       <c r="O35" s="50"/>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A36" s="21"/>
       <c r="B36" s="35"/>
       <c r="C36" s="36"/>
@@ -1660,7 +1660,7 @@
       <c r="N36" s="28"/>
       <c r="O36" s="50"/>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A37" s="21"/>
       <c r="B37" s="35"/>
       <c r="C37" s="36"/>
@@ -1677,7 +1677,7 @@
       <c r="N37" s="28"/>
       <c r="O37" s="50"/>
     </row>
-    <row r="38" spans="1:15" ht="15" customHeight="1">
+    <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="21"/>
       <c r="B38" s="35"/>
       <c r="C38" s="36"/>
@@ -1694,7 +1694,7 @@
       <c r="N38" s="28"/>
       <c r="O38" s="50"/>
     </row>
-    <row r="39" spans="1:15" ht="15" customHeight="1">
+    <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="21"/>
       <c r="B39" s="35"/>
       <c r="C39" s="36"/>
@@ -1711,7 +1711,7 @@
       <c r="N39" s="28"/>
       <c r="O39" s="50"/>
     </row>
-    <row r="40" spans="1:15" ht="15" customHeight="1">
+    <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="21"/>
       <c r="B40" s="35"/>
       <c r="C40" s="36"/>
@@ -1728,7 +1728,7 @@
       <c r="N40" s="28"/>
       <c r="O40" s="50"/>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A41" s="21"/>
       <c r="B41" s="35"/>
       <c r="C41" s="36"/>
@@ -1745,7 +1745,7 @@
       <c r="N41" s="28"/>
       <c r="O41" s="50"/>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A42" s="21"/>
       <c r="B42" s="35"/>
       <c r="C42" s="36"/>
@@ -1762,7 +1762,7 @@
       <c r="N42" s="28"/>
       <c r="O42" s="50"/>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A43" s="21"/>
       <c r="B43" s="35"/>
       <c r="C43" s="36"/>
@@ -1779,7 +1779,7 @@
       <c r="N43" s="28"/>
       <c r="O43" s="50"/>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A44" s="21"/>
       <c r="B44" s="35"/>
       <c r="C44" s="36"/>
@@ -1796,7 +1796,7 @@
       <c r="N44" s="28"/>
       <c r="O44" s="50"/>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A45" s="21"/>
       <c r="B45" s="35"/>
       <c r="C45" s="36"/>
@@ -1813,7 +1813,7 @@
       <c r="N45" s="28"/>
       <c r="O45" s="50"/>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A46" s="21"/>
       <c r="B46" s="35"/>
       <c r="C46" s="36"/>
@@ -1830,7 +1830,7 @@
       <c r="N46" s="28"/>
       <c r="O46" s="50"/>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A47" s="21"/>
       <c r="B47" s="35"/>
       <c r="C47" s="36"/>
@@ -1847,7 +1847,7 @@
       <c r="N47" s="28"/>
       <c r="O47" s="50"/>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A48" s="21"/>
       <c r="B48" s="35"/>
       <c r="C48" s="36"/>
@@ -1864,7 +1864,7 @@
       <c r="N48" s="28"/>
       <c r="O48" s="50"/>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A49" s="21"/>
       <c r="B49" s="35"/>
       <c r="C49" s="36"/>
@@ -1881,7 +1881,7 @@
       <c r="N49" s="28"/>
       <c r="O49" s="50"/>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A50" s="21"/>
       <c r="B50" s="35"/>
       <c r="C50" s="36"/>
@@ -1898,7 +1898,7 @@
       <c r="N50" s="28"/>
       <c r="O50" s="50"/>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A51" s="21"/>
       <c r="B51" s="35"/>
       <c r="C51" s="36"/>
@@ -1915,7 +1915,7 @@
       <c r="N51" s="28"/>
       <c r="O51" s="50"/>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A52" s="21"/>
       <c r="B52" s="35"/>
       <c r="C52" s="36"/>
@@ -1932,7 +1932,7 @@
       <c r="N52" s="28"/>
       <c r="O52" s="50"/>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A53" s="21"/>
       <c r="B53" s="35"/>
       <c r="C53" s="36"/>
@@ -1949,7 +1949,7 @@
       <c r="N53" s="28"/>
       <c r="O53" s="50"/>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A54" s="21"/>
       <c r="B54" s="35"/>
       <c r="C54" s="36"/>
@@ -1966,7 +1966,7 @@
       <c r="N54" s="28"/>
       <c r="O54" s="50"/>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A55" s="21"/>
       <c r="B55" s="35"/>
       <c r="C55" s="36"/>
@@ -1983,7 +1983,7 @@
       <c r="N55" s="28"/>
       <c r="O55" s="50"/>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A56" s="21"/>
       <c r="B56" s="35"/>
       <c r="C56" s="36"/>
@@ -2000,7 +2000,7 @@
       <c r="N56" s="28"/>
       <c r="O56" s="50"/>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A57" s="21"/>
       <c r="B57" s="35"/>
       <c r="C57" s="36"/>
@@ -2017,7 +2017,7 @@
       <c r="N57" s="28"/>
       <c r="O57" s="50"/>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A58" s="21"/>
       <c r="B58" s="35"/>
       <c r="C58" s="36"/>
@@ -2034,7 +2034,7 @@
       <c r="N58" s="28"/>
       <c r="O58" s="50"/>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A59" s="21"/>
       <c r="B59" s="35"/>
       <c r="C59" s="36"/>
@@ -2051,7 +2051,7 @@
       <c r="N59" s="28"/>
       <c r="O59" s="50"/>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A60" s="21"/>
       <c r="B60" s="35"/>
       <c r="C60" s="36"/>
@@ -2068,7 +2068,7 @@
       <c r="N60" s="28"/>
       <c r="O60" s="50"/>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A61" s="21"/>
       <c r="B61" s="35"/>
       <c r="C61" s="36"/>
@@ -2085,7 +2085,7 @@
       <c r="N61" s="28"/>
       <c r="O61" s="50"/>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A62" s="21"/>
       <c r="B62" s="35"/>
       <c r="C62" s="36"/>
@@ -2102,7 +2102,7 @@
       <c r="N62" s="28"/>
       <c r="O62" s="50"/>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A63" s="21"/>
       <c r="B63" s="35"/>
       <c r="C63" s="36"/>
@@ -2119,7 +2119,7 @@
       <c r="N63" s="28"/>
       <c r="O63" s="50"/>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A64" s="21"/>
       <c r="B64" s="35"/>
       <c r="C64" s="36"/>
@@ -2136,7 +2136,7 @@
       <c r="N64" s="28"/>
       <c r="O64" s="50"/>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A65" s="21"/>
       <c r="B65" s="35"/>
       <c r="C65" s="36"/>
@@ -2153,7 +2153,7 @@
       <c r="N65" s="28"/>
       <c r="O65" s="50"/>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A66" s="21"/>
       <c r="B66" s="35"/>
       <c r="C66" s="36"/>
@@ -2170,7 +2170,7 @@
       <c r="N66" s="28"/>
       <c r="O66" s="50"/>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A67" s="21"/>
       <c r="B67" s="35"/>
       <c r="C67" s="36"/>
@@ -2187,7 +2187,7 @@
       <c r="N67" s="28"/>
       <c r="O67" s="50"/>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A68" s="21"/>
       <c r="B68" s="35"/>
       <c r="C68" s="36"/>
@@ -2204,7 +2204,7 @@
       <c r="N68" s="28"/>
       <c r="O68" s="50"/>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A69" s="21"/>
       <c r="B69" s="35"/>
       <c r="C69" s="36"/>
@@ -2221,7 +2221,7 @@
       <c r="N69" s="28"/>
       <c r="O69" s="50"/>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A70" s="21"/>
       <c r="B70" s="35"/>
       <c r="C70" s="36"/>
@@ -2238,7 +2238,7 @@
       <c r="N70" s="28"/>
       <c r="O70" s="50"/>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A71" s="21"/>
       <c r="B71" s="35"/>
       <c r="C71" s="36"/>
@@ -2255,7 +2255,7 @@
       <c r="N71" s="28"/>
       <c r="O71" s="50"/>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A72" s="21"/>
       <c r="B72" s="35"/>
       <c r="C72" s="36"/>
@@ -2272,7 +2272,7 @@
       <c r="N72" s="28"/>
       <c r="O72" s="50"/>
     </row>
-    <row r="73" spans="1:15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A73" s="21"/>
       <c r="B73" s="35"/>
       <c r="C73" s="36"/>
@@ -2289,7 +2289,7 @@
       <c r="N73" s="28"/>
       <c r="O73" s="50"/>
     </row>
-    <row r="74" spans="1:15">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A74" s="21"/>
       <c r="B74" s="35"/>
       <c r="C74" s="36"/>
@@ -2306,7 +2306,7 @@
       <c r="N74" s="28"/>
       <c r="O74" s="50"/>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A75" s="21"/>
       <c r="B75" s="35"/>
       <c r="C75" s="36"/>
@@ -2323,7 +2323,7 @@
       <c r="N75" s="28"/>
       <c r="O75" s="50"/>
     </row>
-    <row r="76" spans="1:15">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A76" s="21"/>
       <c r="B76" s="35"/>
       <c r="C76" s="36"/>
@@ -2340,7 +2340,7 @@
       <c r="N76" s="28"/>
       <c r="O76" s="50"/>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A77" s="21"/>
       <c r="B77" s="35"/>
       <c r="C77" s="36"/>
@@ -2357,7 +2357,7 @@
       <c r="N77" s="28"/>
       <c r="O77" s="50"/>
     </row>
-    <row r="78" spans="1:15">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A78" s="21"/>
       <c r="B78" s="35"/>
       <c r="C78" s="36"/>
@@ -2374,7 +2374,7 @@
       <c r="N78" s="28"/>
       <c r="O78" s="50"/>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A79" s="21"/>
       <c r="B79" s="35"/>
       <c r="C79" s="36"/>
@@ -2391,7 +2391,7 @@
       <c r="N79" s="28"/>
       <c r="O79" s="50"/>
     </row>
-    <row r="80" spans="1:15">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A80" s="21"/>
       <c r="B80" s="35"/>
       <c r="C80" s="36"/>
@@ -2408,7 +2408,7 @@
       <c r="N80" s="28"/>
       <c r="O80" s="50"/>
     </row>
-    <row r="81" spans="1:15">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A81" s="21"/>
       <c r="B81" s="35"/>
       <c r="C81" s="36"/>
@@ -2425,7 +2425,7 @@
       <c r="N81" s="28"/>
       <c r="O81" s="50"/>
     </row>
-    <row r="82" spans="1:15">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A82" s="21"/>
       <c r="B82" s="35"/>
       <c r="C82" s="36"/>
@@ -2442,7 +2442,7 @@
       <c r="N82" s="28"/>
       <c r="O82" s="50"/>
     </row>
-    <row r="83" spans="1:15">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A83" s="21"/>
       <c r="B83" s="35"/>
       <c r="C83" s="36"/>
@@ -2459,7 +2459,7 @@
       <c r="N83" s="28"/>
       <c r="O83" s="50"/>
     </row>
-    <row r="84" spans="1:15">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A84" s="21"/>
       <c r="B84" s="35"/>
       <c r="C84" s="36"/>
@@ -2476,7 +2476,7 @@
       <c r="N84" s="28"/>
       <c r="O84" s="50"/>
     </row>
-    <row r="85" spans="1:15">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A85" s="21"/>
       <c r="B85" s="35"/>
       <c r="C85" s="36"/>
@@ -2493,7 +2493,7 @@
       <c r="N85" s="28"/>
       <c r="O85" s="50"/>
     </row>
-    <row r="86" spans="1:15">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A86" s="21"/>
       <c r="B86" s="35"/>
       <c r="C86" s="36"/>
@@ -2510,7 +2510,7 @@
       <c r="N86" s="28"/>
       <c r="O86" s="50"/>
     </row>
-    <row r="87" spans="1:15">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A87" s="21"/>
       <c r="B87" s="35"/>
       <c r="C87" s="36"/>
@@ -2527,7 +2527,7 @@
       <c r="N87" s="28"/>
       <c r="O87" s="50"/>
     </row>
-    <row r="88" spans="1:15">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A88" s="21"/>
       <c r="B88" s="35"/>
       <c r="C88" s="36"/>
@@ -2544,7 +2544,7 @@
       <c r="N88" s="28"/>
       <c r="O88" s="50"/>
     </row>
-    <row r="89" spans="1:15">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A89" s="21"/>
       <c r="B89" s="35"/>
       <c r="C89" s="36"/>
@@ -2561,7 +2561,7 @@
       <c r="N89" s="28"/>
       <c r="O89" s="50"/>
     </row>
-    <row r="90" spans="1:15">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A90" s="21"/>
       <c r="B90" s="35"/>
       <c r="C90" s="36"/>
@@ -2578,7 +2578,7 @@
       <c r="N90" s="28"/>
       <c r="O90" s="50"/>
     </row>
-    <row r="91" spans="1:15">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A91" s="21"/>
       <c r="B91" s="35"/>
       <c r="C91" s="36"/>
@@ -2595,7 +2595,7 @@
       <c r="N91" s="28"/>
       <c r="O91" s="50"/>
     </row>
-    <row r="92" spans="1:15">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A92" s="21"/>
       <c r="B92" s="35"/>
       <c r="C92" s="36"/>
@@ -2612,7 +2612,7 @@
       <c r="N92" s="28"/>
       <c r="O92" s="50"/>
     </row>
-    <row r="93" spans="1:15">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A93" s="21"/>
       <c r="B93" s="35"/>
       <c r="C93" s="36"/>
@@ -2629,7 +2629,7 @@
       <c r="N93" s="28"/>
       <c r="O93" s="50"/>
     </row>
-    <row r="94" spans="1:15">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A94" s="21"/>
       <c r="B94" s="35"/>
       <c r="C94" s="36"/>
@@ -2646,7 +2646,7 @@
       <c r="N94" s="28"/>
       <c r="O94" s="50"/>
     </row>
-    <row r="95" spans="1:15">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A95" s="21"/>
       <c r="B95" s="35"/>
       <c r="C95" s="36"/>
@@ -2663,7 +2663,7 @@
       <c r="N95" s="28"/>
       <c r="O95" s="50"/>
     </row>
-    <row r="96" spans="1:15">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A96" s="21"/>
       <c r="B96" s="35"/>
       <c r="C96" s="36"/>
@@ -2680,7 +2680,7 @@
       <c r="N96" s="28"/>
       <c r="O96" s="50"/>
     </row>
-    <row r="97" spans="1:15">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A97" s="21"/>
       <c r="B97" s="35"/>
       <c r="C97" s="36"/>
@@ -2697,7 +2697,7 @@
       <c r="N97" s="28"/>
       <c r="O97" s="50"/>
     </row>
-    <row r="98" spans="1:15">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A98" s="21"/>
       <c r="B98" s="35"/>
       <c r="C98" s="36"/>
@@ -2714,7 +2714,7 @@
       <c r="N98" s="28"/>
       <c r="O98" s="50"/>
     </row>
-    <row r="99" spans="1:15">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A99" s="21"/>
       <c r="B99" s="35"/>
       <c r="C99" s="36"/>
@@ -2731,7 +2731,7 @@
       <c r="N99" s="28"/>
       <c r="O99" s="50"/>
     </row>
-    <row r="100" spans="1:15">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A100" s="21"/>
       <c r="B100" s="35"/>
       <c r="C100" s="36"/>
@@ -2748,7 +2748,7 @@
       <c r="N100" s="28"/>
       <c r="O100" s="50"/>
     </row>
-    <row r="101" spans="1:15">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A101" s="21"/>
       <c r="B101" s="35"/>
       <c r="C101" s="36"/>
@@ -2765,7 +2765,7 @@
       <c r="N101" s="28"/>
       <c r="O101" s="50"/>
     </row>
-    <row r="102" spans="1:15">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A102" s="21"/>
       <c r="B102" s="35"/>
       <c r="C102" s="36"/>
@@ -2782,7 +2782,7 @@
       <c r="N102" s="28"/>
       <c r="O102" s="50"/>
     </row>
-    <row r="103" spans="1:15">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A103" s="21"/>
       <c r="B103" s="35"/>
       <c r="C103" s="36"/>
@@ -2799,7 +2799,7 @@
       <c r="N103" s="28"/>
       <c r="O103" s="50"/>
     </row>
-    <row r="104" spans="1:15">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A104" s="21"/>
       <c r="B104" s="35"/>
       <c r="C104" s="36"/>
@@ -2816,7 +2816,7 @@
       <c r="N104" s="28"/>
       <c r="O104" s="50"/>
     </row>
-    <row r="105" spans="1:15">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A105" s="21"/>
       <c r="B105" s="35"/>
       <c r="C105" s="36"/>
@@ -2833,7 +2833,7 @@
       <c r="N105" s="28"/>
       <c r="O105" s="50"/>
     </row>
-    <row r="106" spans="1:15">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A106" s="21"/>
       <c r="B106" s="35"/>
       <c r="C106" s="36"/>
@@ -2850,7 +2850,7 @@
       <c r="N106" s="28"/>
       <c r="O106" s="50"/>
     </row>
-    <row r="107" spans="1:15">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A107" s="21"/>
       <c r="B107" s="35"/>
       <c r="C107" s="36"/>
@@ -2867,7 +2867,7 @@
       <c r="N107" s="28"/>
       <c r="O107" s="50"/>
     </row>
-    <row r="108" spans="1:15">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A108" s="21"/>
       <c r="B108" s="35"/>
       <c r="C108" s="36"/>
@@ -2884,7 +2884,7 @@
       <c r="N108" s="28"/>
       <c r="O108" s="50"/>
     </row>
-    <row r="109" spans="1:15">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A109" s="21"/>
       <c r="B109" s="35"/>
       <c r="C109" s="36"/>
@@ -2901,7 +2901,7 @@
       <c r="N109" s="28"/>
       <c r="O109" s="50"/>
     </row>
-    <row r="110" spans="1:15">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A110" s="21"/>
       <c r="B110" s="35"/>
       <c r="C110" s="36"/>
@@ -2918,7 +2918,7 @@
       <c r="N110" s="28"/>
       <c r="O110" s="50"/>
     </row>
-    <row r="111" spans="1:15">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A111" s="21"/>
       <c r="B111" s="35"/>
       <c r="C111" s="36"/>
@@ -2935,7 +2935,7 @@
       <c r="N111" s="28"/>
       <c r="O111" s="50"/>
     </row>
-    <row r="112" spans="1:15">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A112" s="21"/>
       <c r="B112" s="35"/>
       <c r="C112" s="36"/>
@@ -2952,7 +2952,7 @@
       <c r="N112" s="28"/>
       <c r="O112" s="50"/>
     </row>
-    <row r="113" spans="1:15">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A113" s="21"/>
       <c r="B113" s="35"/>
       <c r="C113" s="36"/>
@@ -2969,7 +2969,7 @@
       <c r="N113" s="28"/>
       <c r="O113" s="50"/>
     </row>
-    <row r="114" spans="1:15">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A114" s="21"/>
       <c r="B114" s="35"/>
       <c r="C114" s="36"/>
@@ -2986,7 +2986,7 @@
       <c r="N114" s="28"/>
       <c r="O114" s="50"/>
     </row>
-    <row r="115" spans="1:15">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A115" s="21"/>
       <c r="B115" s="35"/>
       <c r="C115" s="36"/>
@@ -3003,7 +3003,7 @@
       <c r="N115" s="28"/>
       <c r="O115" s="50"/>
     </row>
-    <row r="116" spans="1:15">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A116" s="21"/>
       <c r="B116" s="35"/>
       <c r="C116" s="36"/>
@@ -3020,7 +3020,7 @@
       <c r="N116" s="28"/>
       <c r="O116" s="50"/>
     </row>
-    <row r="117" spans="1:15">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A117" s="21"/>
       <c r="B117" s="35"/>
       <c r="C117" s="36"/>
@@ -3037,7 +3037,7 @@
       <c r="N117" s="28"/>
       <c r="O117" s="50"/>
     </row>
-    <row r="118" spans="1:15">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A118" s="21"/>
       <c r="B118" s="35"/>
       <c r="C118" s="36"/>
@@ -3054,7 +3054,7 @@
       <c r="N118" s="28"/>
       <c r="O118" s="50"/>
     </row>
-    <row r="119" spans="1:15">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A119" s="21"/>
       <c r="B119" s="35"/>
       <c r="C119" s="36"/>
@@ -3071,7 +3071,7 @@
       <c r="N119" s="28"/>
       <c r="O119" s="50"/>
     </row>
-    <row r="120" spans="1:15">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A120" s="21"/>
       <c r="B120" s="35"/>
       <c r="C120" s="36"/>
@@ -3088,7 +3088,7 @@
       <c r="N120" s="28"/>
       <c r="O120" s="50"/>
     </row>
-    <row r="121" spans="1:15">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A121" s="21"/>
       <c r="B121" s="35"/>
       <c r="C121" s="36"/>
@@ -3105,7 +3105,7 @@
       <c r="N121" s="28"/>
       <c r="O121" s="50"/>
     </row>
-    <row r="122" spans="1:15">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A122" s="21"/>
       <c r="B122" s="35"/>
       <c r="C122" s="36"/>
@@ -3122,7 +3122,7 @@
       <c r="N122" s="28"/>
       <c r="O122" s="50"/>
     </row>
-    <row r="123" spans="1:15">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A123" s="21"/>
       <c r="B123" s="35"/>
       <c r="C123" s="36"/>
@@ -3139,7 +3139,7 @@
       <c r="N123" s="28"/>
       <c r="O123" s="50"/>
     </row>
-    <row r="124" spans="1:15">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A124" s="21"/>
       <c r="B124" s="35"/>
       <c r="C124" s="36"/>
@@ -3156,7 +3156,7 @@
       <c r="N124" s="28"/>
       <c r="O124" s="50"/>
     </row>
-    <row r="125" spans="1:15">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A125" s="21"/>
       <c r="B125" s="35"/>
       <c r="C125" s="36"/>
@@ -3173,7 +3173,7 @@
       <c r="N125" s="28"/>
       <c r="O125" s="50"/>
     </row>
-    <row r="126" spans="1:15">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A126" s="21"/>
       <c r="B126" s="35"/>
       <c r="C126" s="36"/>
@@ -3190,7 +3190,7 @@
       <c r="N126" s="28"/>
       <c r="O126" s="50"/>
     </row>
-    <row r="127" spans="1:15">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A127" s="21"/>
       <c r="B127" s="35"/>
       <c r="C127" s="36"/>
@@ -3207,7 +3207,7 @@
       <c r="N127" s="28"/>
       <c r="O127" s="50"/>
     </row>
-    <row r="128" spans="1:15">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A128" s="21"/>
       <c r="B128" s="35"/>
       <c r="C128" s="36"/>
@@ -3224,7 +3224,7 @@
       <c r="N128" s="28"/>
       <c r="O128" s="50"/>
     </row>
-    <row r="129" spans="1:15">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A129" s="21"/>
       <c r="B129" s="35"/>
       <c r="C129" s="36"/>
@@ -3241,7 +3241,7 @@
       <c r="N129" s="28"/>
       <c r="O129" s="50"/>
     </row>
-    <row r="130" spans="1:15">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A130" s="21"/>
       <c r="B130" s="35"/>
       <c r="C130" s="36"/>
@@ -3258,7 +3258,7 @@
       <c r="N130" s="28"/>
       <c r="O130" s="50"/>
     </row>
-    <row r="131" spans="1:15">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A131" s="21"/>
       <c r="B131" s="35"/>
       <c r="C131" s="36"/>
@@ -3275,7 +3275,7 @@
       <c r="N131" s="28"/>
       <c r="O131" s="50"/>
     </row>
-    <row r="132" spans="1:15">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A132" s="21"/>
       <c r="B132" s="35"/>
       <c r="C132" s="36"/>
@@ -3292,7 +3292,7 @@
       <c r="N132" s="28"/>
       <c r="O132" s="50"/>
     </row>
-    <row r="133" spans="1:15">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A133" s="21"/>
       <c r="B133" s="35"/>
       <c r="C133" s="36"/>
@@ -3309,7 +3309,7 @@
       <c r="N133" s="28"/>
       <c r="O133" s="50"/>
     </row>
-    <row r="134" spans="1:15">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A134" s="21"/>
       <c r="B134" s="35"/>
       <c r="C134" s="36"/>
@@ -3326,7 +3326,7 @@
       <c r="N134" s="28"/>
       <c r="O134" s="50"/>
     </row>
-    <row r="135" spans="1:15">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A135" s="21"/>
       <c r="B135" s="35"/>
       <c r="C135" s="36"/>
@@ -3343,7 +3343,7 @@
       <c r="N135" s="28"/>
       <c r="O135" s="50"/>
     </row>
-    <row r="136" spans="1:15">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A136" s="21"/>
       <c r="B136" s="35"/>
       <c r="C136" s="36"/>
@@ -3360,7 +3360,7 @@
       <c r="N136" s="28"/>
       <c r="O136" s="50"/>
     </row>
-    <row r="137" spans="1:15">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A137" s="21"/>
       <c r="B137" s="35"/>
       <c r="C137" s="36"/>
@@ -3377,7 +3377,7 @@
       <c r="N137" s="28"/>
       <c r="O137" s="50"/>
     </row>
-    <row r="138" spans="1:15">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A138" s="21"/>
       <c r="B138" s="35"/>
       <c r="C138" s="36"/>
@@ -3394,7 +3394,7 @@
       <c r="N138" s="28"/>
       <c r="O138" s="50"/>
     </row>
-    <row r="139" spans="1:15">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A139" s="21"/>
       <c r="B139" s="35"/>
       <c r="C139" s="36"/>
@@ -3411,7 +3411,7 @@
       <c r="N139" s="28"/>
       <c r="O139" s="50"/>
     </row>
-    <row r="140" spans="1:15">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A140" s="21"/>
       <c r="B140" s="35"/>
       <c r="C140" s="36"/>
@@ -3428,7 +3428,7 @@
       <c r="N140" s="28"/>
       <c r="O140" s="50"/>
     </row>
-    <row r="141" spans="1:15">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A141" s="21"/>
       <c r="B141" s="35"/>
       <c r="C141" s="36"/>
@@ -3445,7 +3445,7 @@
       <c r="N141" s="28"/>
       <c r="O141" s="50"/>
     </row>
-    <row r="142" spans="1:15">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A142" s="21"/>
       <c r="B142" s="35"/>
       <c r="C142" s="36"/>
@@ -3462,7 +3462,7 @@
       <c r="N142" s="28"/>
       <c r="O142" s="50"/>
     </row>
-    <row r="143" spans="1:15">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A143" s="21"/>
       <c r="B143" s="35"/>
       <c r="C143" s="36"/>
@@ -3479,7 +3479,7 @@
       <c r="N143" s="28"/>
       <c r="O143" s="50"/>
     </row>
-    <row r="144" spans="1:15">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A144" s="21"/>
       <c r="B144" s="35"/>
       <c r="C144" s="36"/>
@@ -3496,7 +3496,7 @@
       <c r="N144" s="28"/>
       <c r="O144" s="50"/>
     </row>
-    <row r="145" spans="1:15">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A145" s="21"/>
       <c r="B145" s="35"/>
       <c r="C145" s="36"/>
@@ -3513,7 +3513,7 @@
       <c r="N145" s="28"/>
       <c r="O145" s="50"/>
     </row>
-    <row r="146" spans="1:15">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A146" s="21"/>
       <c r="B146" s="35"/>
       <c r="C146" s="36"/>
@@ -3530,7 +3530,7 @@
       <c r="N146" s="28"/>
       <c r="O146" s="50"/>
     </row>
-    <row r="147" spans="1:15">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A147" s="21"/>
       <c r="B147" s="35"/>
       <c r="C147" s="36"/>
@@ -3547,7 +3547,7 @@
       <c r="N147" s="28"/>
       <c r="O147" s="50"/>
     </row>
-    <row r="148" spans="1:15">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A148" s="21"/>
       <c r="B148" s="35"/>
       <c r="C148" s="36"/>
@@ -3564,7 +3564,7 @@
       <c r="N148" s="28"/>
       <c r="O148" s="50"/>
     </row>
-    <row r="149" spans="1:15">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A149" s="21"/>
       <c r="B149" s="35"/>
       <c r="C149" s="36"/>
@@ -3581,7 +3581,7 @@
       <c r="N149" s="28"/>
       <c r="O149" s="50"/>
     </row>
-    <row r="150" spans="1:15">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A150" s="21"/>
       <c r="B150" s="35"/>
       <c r="C150" s="36"/>
@@ -3598,7 +3598,7 @@
       <c r="N150" s="28"/>
       <c r="O150" s="50"/>
     </row>
-    <row r="151" spans="1:15">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A151" s="21"/>
       <c r="B151" s="35"/>
       <c r="C151" s="36"/>
@@ -3615,7 +3615,7 @@
       <c r="N151" s="28"/>
       <c r="O151" s="50"/>
     </row>
-    <row r="152" spans="1:15">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A152" s="21"/>
       <c r="B152" s="35"/>
       <c r="C152" s="36"/>
@@ -3632,7 +3632,7 @@
       <c r="N152" s="28"/>
       <c r="O152" s="50"/>
     </row>
-    <row r="153" spans="1:15">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A153" s="21"/>
       <c r="B153" s="35"/>
       <c r="C153" s="36"/>
@@ -3649,7 +3649,7 @@
       <c r="N153" s="28"/>
       <c r="O153" s="50"/>
     </row>
-    <row r="154" spans="1:15">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A154" s="21"/>
       <c r="B154" s="35"/>
       <c r="C154" s="36"/>
@@ -3666,7 +3666,7 @@
       <c r="N154" s="28"/>
       <c r="O154" s="50"/>
     </row>
-    <row r="155" spans="1:15">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A155" s="21"/>
       <c r="B155" s="35"/>
       <c r="C155" s="36"/>
@@ -3683,7 +3683,7 @@
       <c r="N155" s="28"/>
       <c r="O155" s="50"/>
     </row>
-    <row r="156" spans="1:15">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A156" s="21"/>
       <c r="B156" s="35"/>
       <c r="C156" s="36"/>
@@ -3700,7 +3700,7 @@
       <c r="N156" s="28"/>
       <c r="O156" s="50"/>
     </row>
-    <row r="157" spans="1:15">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A157" s="21"/>
       <c r="B157" s="35"/>
       <c r="C157" s="36"/>
@@ -3717,7 +3717,7 @@
       <c r="N157" s="28"/>
       <c r="O157" s="50"/>
     </row>
-    <row r="158" spans="1:15">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A158" s="21"/>
       <c r="B158" s="35"/>
       <c r="C158" s="36"/>
@@ -3734,7 +3734,7 @@
       <c r="N158" s="28"/>
       <c r="O158" s="50"/>
     </row>
-    <row r="159" spans="1:15">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A159" s="21"/>
       <c r="B159" s="35"/>
       <c r="C159" s="36"/>
@@ -3751,7 +3751,7 @@
       <c r="N159" s="28"/>
       <c r="O159" s="50"/>
     </row>
-    <row r="160" spans="1:15">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A160" s="21"/>
       <c r="B160" s="35"/>
       <c r="C160" s="36"/>
@@ -3768,7 +3768,7 @@
       <c r="N160" s="28"/>
       <c r="O160" s="50"/>
     </row>
-    <row r="161" spans="1:15">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A161" s="21"/>
       <c r="B161" s="35"/>
       <c r="C161" s="36"/>
@@ -3785,7 +3785,7 @@
       <c r="N161" s="28"/>
       <c r="O161" s="50"/>
     </row>
-    <row r="162" spans="1:15">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A162" s="21"/>
       <c r="B162" s="35"/>
       <c r="C162" s="36"/>
@@ -3802,7 +3802,7 @@
       <c r="N162" s="28"/>
       <c r="O162" s="50"/>
     </row>
-    <row r="163" spans="1:15">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A163" s="21"/>
       <c r="B163" s="35"/>
       <c r="C163" s="36"/>
@@ -3819,7 +3819,7 @@
       <c r="N163" s="28"/>
       <c r="O163" s="50"/>
     </row>
-    <row r="164" spans="1:15">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A164" s="21"/>
       <c r="B164" s="35"/>
       <c r="C164" s="36"/>
@@ -3836,7 +3836,7 @@
       <c r="N164" s="28"/>
       <c r="O164" s="50"/>
     </row>
-    <row r="165" spans="1:15">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A165" s="21"/>
       <c r="B165" s="35"/>
       <c r="C165" s="36"/>
@@ -3853,7 +3853,7 @@
       <c r="N165" s="28"/>
       <c r="O165" s="50"/>
     </row>
-    <row r="166" spans="1:15">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A166" s="21"/>
       <c r="B166" s="35"/>
       <c r="C166" s="36"/>
@@ -3870,7 +3870,7 @@
       <c r="N166" s="28"/>
       <c r="O166" s="50"/>
     </row>
-    <row r="167" spans="1:15">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A167" s="21"/>
       <c r="B167" s="35"/>
       <c r="C167" s="36"/>
@@ -3887,7 +3887,7 @@
       <c r="N167" s="28"/>
       <c r="O167" s="50"/>
     </row>
-    <row r="168" spans="1:15">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A168" s="21"/>
       <c r="B168" s="35"/>
       <c r="C168" s="36"/>
@@ -3904,7 +3904,7 @@
       <c r="N168" s="28"/>
       <c r="O168" s="50"/>
     </row>
-    <row r="169" spans="1:15">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A169" s="21"/>
       <c r="B169" s="35"/>
       <c r="C169" s="36"/>
@@ -3921,7 +3921,7 @@
       <c r="N169" s="28"/>
       <c r="O169" s="50"/>
     </row>
-    <row r="170" spans="1:15">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A170" s="21"/>
       <c r="B170" s="35"/>
       <c r="C170" s="36"/>
@@ -3938,7 +3938,7 @@
       <c r="N170" s="28"/>
       <c r="O170" s="50"/>
     </row>
-    <row r="171" spans="1:15">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A171" s="21"/>
       <c r="B171" s="35"/>
       <c r="C171" s="36"/>
@@ -3955,7 +3955,7 @@
       <c r="N171" s="28"/>
       <c r="O171" s="50"/>
     </row>
-    <row r="172" spans="1:15">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A172" s="21"/>
       <c r="B172" s="35"/>
       <c r="C172" s="36"/>
@@ -3972,7 +3972,7 @@
       <c r="N172" s="28"/>
       <c r="O172" s="50"/>
     </row>
-    <row r="173" spans="1:15">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A173" s="21"/>
       <c r="B173" s="35"/>
       <c r="C173" s="36"/>
@@ -3989,7 +3989,7 @@
       <c r="N173" s="28"/>
       <c r="O173" s="50"/>
     </row>
-    <row r="174" spans="1:15">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A174" s="21"/>
       <c r="B174" s="35"/>
       <c r="C174" s="36"/>
@@ -4006,7 +4006,7 @@
       <c r="N174" s="28"/>
       <c r="O174" s="50"/>
     </row>
-    <row r="175" spans="1:15">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A175" s="21"/>
       <c r="B175" s="35"/>
       <c r="C175" s="36"/>
@@ -4023,7 +4023,7 @@
       <c r="N175" s="28"/>
       <c r="O175" s="50"/>
     </row>
-    <row r="176" spans="1:15">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A176" s="21"/>
       <c r="B176" s="35"/>
       <c r="C176" s="36"/>
@@ -4040,7 +4040,7 @@
       <c r="N176" s="28"/>
       <c r="O176" s="50"/>
     </row>
-    <row r="177" spans="1:15">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A177" s="21"/>
       <c r="B177" s="35"/>
       <c r="C177" s="36"/>
@@ -4057,7 +4057,7 @@
       <c r="N177" s="28"/>
       <c r="O177" s="50"/>
     </row>
-    <row r="178" spans="1:15">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A178" s="21"/>
       <c r="B178" s="35"/>
       <c r="C178" s="36"/>
@@ -4074,7 +4074,7 @@
       <c r="N178" s="28"/>
       <c r="O178" s="50"/>
     </row>
-    <row r="179" spans="1:15">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A179" s="21"/>
       <c r="B179" s="35"/>
       <c r="C179" s="36"/>
@@ -4091,7 +4091,7 @@
       <c r="N179" s="28"/>
       <c r="O179" s="50"/>
     </row>
-    <row r="180" spans="1:15">
+    <row r="180" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A180" s="21"/>
       <c r="B180" s="35"/>
       <c r="C180" s="36"/>
@@ -4108,7 +4108,7 @@
       <c r="N180" s="28"/>
       <c r="O180" s="50"/>
     </row>
-    <row r="181" spans="1:15">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A181" s="21"/>
       <c r="B181" s="35"/>
       <c r="C181" s="36"/>
@@ -4125,7 +4125,7 @@
       <c r="N181" s="28"/>
       <c r="O181" s="50"/>
     </row>
-    <row r="182" spans="1:15">
+    <row r="182" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A182" s="21"/>
       <c r="B182" s="35"/>
       <c r="C182" s="36"/>
@@ -4142,7 +4142,7 @@
       <c r="N182" s="28"/>
       <c r="O182" s="50"/>
     </row>
-    <row r="183" spans="1:15">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A183" s="21"/>
       <c r="B183" s="35"/>
       <c r="C183" s="36"/>
@@ -4159,7 +4159,7 @@
       <c r="N183" s="28"/>
       <c r="O183" s="50"/>
     </row>
-    <row r="184" spans="1:15">
+    <row r="184" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A184" s="21"/>
       <c r="B184" s="35"/>
       <c r="C184" s="36"/>
@@ -4176,7 +4176,7 @@
       <c r="N184" s="28"/>
       <c r="O184" s="50"/>
     </row>
-    <row r="185" spans="1:15">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A185" s="21"/>
       <c r="B185" s="35"/>
       <c r="C185" s="36"/>
@@ -4193,7 +4193,7 @@
       <c r="N185" s="28"/>
       <c r="O185" s="50"/>
     </row>
-    <row r="186" spans="1:15">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A186" s="21"/>
       <c r="B186" s="35"/>
       <c r="C186" s="36"/>
@@ -4210,7 +4210,7 @@
       <c r="N186" s="28"/>
       <c r="O186" s="50"/>
     </row>
-    <row r="187" spans="1:15">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A187" s="21"/>
       <c r="B187" s="35"/>
       <c r="C187" s="36"/>
@@ -4227,7 +4227,7 @@
       <c r="N187" s="28"/>
       <c r="O187" s="50"/>
     </row>
-    <row r="188" spans="1:15">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A188" s="21"/>
       <c r="B188" s="35"/>
       <c r="C188" s="36"/>
@@ -4244,7 +4244,7 @@
       <c r="N188" s="28"/>
       <c r="O188" s="50"/>
     </row>
-    <row r="189" spans="1:15">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A189" s="21"/>
       <c r="B189" s="35"/>
       <c r="C189" s="36"/>
@@ -4261,7 +4261,7 @@
       <c r="N189" s="28"/>
       <c r="O189" s="50"/>
     </row>
-    <row r="190" spans="1:15">
+    <row r="190" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A190" s="21"/>
       <c r="B190" s="35"/>
       <c r="C190" s="36"/>
@@ -4278,7 +4278,7 @@
       <c r="N190" s="28"/>
       <c r="O190" s="50"/>
     </row>
-    <row r="191" spans="1:15">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A191" s="21"/>
       <c r="B191" s="35"/>
       <c r="C191" s="36"/>
@@ -4295,7 +4295,7 @@
       <c r="N191" s="28"/>
       <c r="O191" s="50"/>
     </row>
-    <row r="192" spans="1:15">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A192" s="21"/>
       <c r="B192" s="35"/>
       <c r="C192" s="36"/>
@@ -4312,7 +4312,7 @@
       <c r="N192" s="28"/>
       <c r="O192" s="50"/>
     </row>
-    <row r="193" spans="1:15">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A193" s="21"/>
       <c r="B193" s="35"/>
       <c r="C193" s="36"/>
@@ -4329,7 +4329,7 @@
       <c r="N193" s="28"/>
       <c r="O193" s="50"/>
     </row>
-    <row r="194" spans="1:15">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A194" s="21"/>
       <c r="B194" s="35"/>
       <c r="C194" s="36"/>
@@ -4346,7 +4346,7 @@
       <c r="N194" s="28"/>
       <c r="O194" s="50"/>
     </row>
-    <row r="195" spans="1:15">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A195" s="21"/>
       <c r="B195" s="35"/>
       <c r="C195" s="36"/>
@@ -4363,7 +4363,7 @@
       <c r="N195" s="28"/>
       <c r="O195" s="50"/>
     </row>
-    <row r="196" spans="1:15">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A196" s="21"/>
       <c r="B196" s="35"/>
       <c r="C196" s="36"/>
@@ -4380,7 +4380,7 @@
       <c r="N196" s="28"/>
       <c r="O196" s="50"/>
     </row>
-    <row r="197" spans="1:15">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A197" s="21"/>
       <c r="B197" s="35"/>
       <c r="C197" s="36"/>
@@ -4397,7 +4397,7 @@
       <c r="N197" s="28"/>
       <c r="O197" s="50"/>
     </row>
-    <row r="198" spans="1:15">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A198" s="21"/>
       <c r="B198" s="35"/>
       <c r="C198" s="36"/>
@@ -4414,7 +4414,7 @@
       <c r="N198" s="28"/>
       <c r="O198" s="50"/>
     </row>
-    <row r="199" spans="1:15">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A199" s="21"/>
       <c r="B199" s="35"/>
       <c r="C199" s="36"/>
@@ -4431,7 +4431,7 @@
       <c r="N199" s="28"/>
       <c r="O199" s="50"/>
     </row>
-    <row r="200" spans="1:15">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A200" s="21"/>
       <c r="B200" s="35"/>
       <c r="C200" s="36"/>
@@ -4448,7 +4448,7 @@
       <c r="N200" s="28"/>
       <c r="O200" s="50"/>
     </row>
-    <row r="201" spans="1:15">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A201" s="21"/>
       <c r="B201" s="35"/>
       <c r="C201" s="36"/>
@@ -4465,7 +4465,7 @@
       <c r="N201" s="28"/>
       <c r="O201" s="50"/>
     </row>
-    <row r="202" spans="1:15">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A202" s="21"/>
       <c r="B202" s="35"/>
       <c r="C202" s="36"/>
@@ -4482,7 +4482,7 @@
       <c r="N202" s="28"/>
       <c r="O202" s="50"/>
     </row>
-    <row r="203" spans="1:15">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A203" s="21"/>
       <c r="B203" s="35"/>
       <c r="C203" s="36"/>
@@ -4499,7 +4499,7 @@
       <c r="N203" s="28"/>
       <c r="O203" s="50"/>
     </row>
-    <row r="204" spans="1:15">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A204" s="21"/>
       <c r="B204" s="35"/>
       <c r="C204" s="36"/>
@@ -4516,7 +4516,7 @@
       <c r="N204" s="28"/>
       <c r="O204" s="50"/>
     </row>
-    <row r="205" spans="1:15">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A205" s="21"/>
       <c r="B205" s="35"/>
       <c r="C205" s="36"/>
@@ -4533,7 +4533,7 @@
       <c r="N205" s="28"/>
       <c r="O205" s="50"/>
     </row>
-    <row r="206" spans="1:15">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A206" s="21"/>
       <c r="B206" s="35"/>
       <c r="C206" s="36"/>
@@ -4550,7 +4550,7 @@
       <c r="N206" s="28"/>
       <c r="O206" s="50"/>
     </row>
-    <row r="207" spans="1:15">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A207" s="21"/>
       <c r="B207" s="35"/>
       <c r="C207" s="36"/>
@@ -4567,7 +4567,7 @@
       <c r="N207" s="28"/>
       <c r="O207" s="50"/>
     </row>
-    <row r="208" spans="1:15">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A208" s="21"/>
       <c r="B208" s="35"/>
       <c r="C208" s="36"/>
@@ -4584,7 +4584,7 @@
       <c r="N208" s="28"/>
       <c r="O208" s="50"/>
     </row>
-    <row r="209" spans="1:15">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A209" s="21"/>
       <c r="B209" s="35"/>
       <c r="C209" s="36"/>
@@ -4601,7 +4601,7 @@
       <c r="N209" s="28"/>
       <c r="O209" s="50"/>
     </row>
-    <row r="210" spans="1:15">
+    <row r="210" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A210" s="21"/>
       <c r="B210" s="35"/>
       <c r="C210" s="36"/>
@@ -4618,7 +4618,7 @@
       <c r="N210" s="28"/>
       <c r="O210" s="50"/>
     </row>
-    <row r="211" spans="1:15">
+    <row r="211" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A211" s="21"/>
       <c r="B211" s="35"/>
       <c r="C211" s="36"/>
@@ -4635,7 +4635,7 @@
       <c r="N211" s="28"/>
       <c r="O211" s="50"/>
     </row>
-    <row r="212" spans="1:15">
+    <row r="212" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A212" s="21"/>
       <c r="B212" s="35"/>
       <c r="C212" s="36"/>
@@ -4652,7 +4652,7 @@
       <c r="N212" s="28"/>
       <c r="O212" s="50"/>
     </row>
-    <row r="213" spans="1:15">
+    <row r="213" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A213" s="21"/>
       <c r="B213" s="35"/>
       <c r="C213" s="36"/>
@@ -4669,7 +4669,7 @@
       <c r="N213" s="28"/>
       <c r="O213" s="50"/>
     </row>
-    <row r="214" spans="1:15">
+    <row r="214" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A214" s="21"/>
       <c r="B214" s="35"/>
       <c r="C214" s="36"/>
@@ -4686,7 +4686,7 @@
       <c r="N214" s="28"/>
       <c r="O214" s="50"/>
     </row>
-    <row r="215" spans="1:15">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A215" s="21"/>
       <c r="B215" s="35"/>
       <c r="C215" s="36"/>
@@ -4703,7 +4703,7 @@
       <c r="N215" s="28"/>
       <c r="O215" s="50"/>
     </row>
-    <row r="216" spans="1:15">
+    <row r="216" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A216" s="21"/>
       <c r="B216" s="35"/>
       <c r="C216" s="36"/>
@@ -4720,7 +4720,7 @@
       <c r="N216" s="28"/>
       <c r="O216" s="50"/>
     </row>
-    <row r="217" spans="1:15">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A217" s="21"/>
       <c r="B217" s="35"/>
       <c r="C217" s="36"/>
@@ -4737,7 +4737,7 @@
       <c r="N217" s="28"/>
       <c r="O217" s="50"/>
     </row>
-    <row r="218" spans="1:15">
+    <row r="218" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A218" s="21"/>
       <c r="B218" s="35"/>
       <c r="C218" s="36"/>
@@ -4754,7 +4754,7 @@
       <c r="N218" s="28"/>
       <c r="O218" s="50"/>
     </row>
-    <row r="219" spans="1:15">
+    <row r="219" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A219" s="21"/>
       <c r="B219" s="35"/>
       <c r="C219" s="36"/>
@@ -4771,7 +4771,7 @@
       <c r="N219" s="28"/>
       <c r="O219" s="50"/>
     </row>
-    <row r="220" spans="1:15">
+    <row r="220" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A220" s="21"/>
       <c r="B220" s="35"/>
       <c r="C220" s="36"/>
@@ -4788,7 +4788,7 @@
       <c r="N220" s="28"/>
       <c r="O220" s="50"/>
     </row>
-    <row r="221" spans="1:15">
+    <row r="221" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A221" s="21"/>
       <c r="B221" s="35"/>
       <c r="C221" s="36"/>
@@ -4805,7 +4805,7 @@
       <c r="N221" s="28"/>
       <c r="O221" s="50"/>
     </row>
-    <row r="222" spans="1:15">
+    <row r="222" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A222" s="21"/>
       <c r="B222" s="35"/>
       <c r="C222" s="36"/>
@@ -4822,7 +4822,7 @@
       <c r="N222" s="28"/>
       <c r="O222" s="50"/>
     </row>
-    <row r="223" spans="1:15">
+    <row r="223" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A223" s="21"/>
       <c r="B223" s="35"/>
       <c r="C223" s="36"/>
@@ -4839,7 +4839,7 @@
       <c r="N223" s="28"/>
       <c r="O223" s="50"/>
     </row>
-    <row r="224" spans="1:15">
+    <row r="224" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A224" s="21"/>
       <c r="B224" s="35"/>
       <c r="C224" s="36"/>
@@ -4856,7 +4856,7 @@
       <c r="N224" s="28"/>
       <c r="O224" s="50"/>
     </row>
-    <row r="225" spans="1:15">
+    <row r="225" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A225" s="21"/>
       <c r="B225" s="35"/>
       <c r="C225" s="36"/>
@@ -4873,7 +4873,7 @@
       <c r="N225" s="28"/>
       <c r="O225" s="50"/>
     </row>
-    <row r="226" spans="1:15">
+    <row r="226" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A226" s="21"/>
       <c r="B226" s="35"/>
       <c r="C226" s="36"/>
@@ -4890,7 +4890,7 @@
       <c r="N226" s="28"/>
       <c r="O226" s="50"/>
     </row>
-    <row r="227" spans="1:15">
+    <row r="227" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A227" s="21"/>
       <c r="B227" s="35"/>
       <c r="C227" s="36"/>
@@ -4907,7 +4907,7 @@
       <c r="N227" s="28"/>
       <c r="O227" s="50"/>
     </row>
-    <row r="228" spans="1:15">
+    <row r="228" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A228" s="21"/>
       <c r="B228" s="35"/>
       <c r="C228" s="36"/>
@@ -4924,7 +4924,7 @@
       <c r="N228" s="28"/>
       <c r="O228" s="50"/>
     </row>
-    <row r="229" spans="1:15">
+    <row r="229" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A229" s="21"/>
       <c r="B229" s="35"/>
       <c r="C229" s="36"/>
@@ -4941,7 +4941,7 @@
       <c r="N229" s="28"/>
       <c r="O229" s="50"/>
     </row>
-    <row r="230" spans="1:15">
+    <row r="230" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A230" s="21"/>
       <c r="B230" s="35"/>
       <c r="C230" s="36"/>
@@ -4958,7 +4958,7 @@
       <c r="N230" s="28"/>
       <c r="O230" s="50"/>
     </row>
-    <row r="231" spans="1:15">
+    <row r="231" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A231" s="21"/>
       <c r="B231" s="35"/>
       <c r="C231" s="36"/>
@@ -4975,7 +4975,7 @@
       <c r="N231" s="28"/>
       <c r="O231" s="50"/>
     </row>
-    <row r="232" spans="1:15">
+    <row r="232" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A232" s="21"/>
       <c r="B232" s="35"/>
       <c r="C232" s="36"/>
@@ -4992,7 +4992,7 @@
       <c r="N232" s="28"/>
       <c r="O232" s="50"/>
     </row>
-    <row r="233" spans="1:15">
+    <row r="233" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A233" s="21"/>
       <c r="B233" s="35"/>
       <c r="C233" s="36"/>
@@ -5009,7 +5009,7 @@
       <c r="N233" s="28"/>
       <c r="O233" s="50"/>
     </row>
-    <row r="234" spans="1:15">
+    <row r="234" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A234" s="21"/>
       <c r="B234" s="35"/>
       <c r="C234" s="36"/>
@@ -5026,7 +5026,7 @@
       <c r="N234" s="28"/>
       <c r="O234" s="50"/>
     </row>
-    <row r="235" spans="1:15">
+    <row r="235" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A235" s="21"/>
       <c r="B235" s="35"/>
       <c r="C235" s="36"/>
@@ -5043,7 +5043,7 @@
       <c r="N235" s="28"/>
       <c r="O235" s="50"/>
     </row>
-    <row r="236" spans="1:15">
+    <row r="236" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A236" s="21"/>
       <c r="B236" s="35"/>
       <c r="C236" s="36"/>
@@ -5060,7 +5060,7 @@
       <c r="N236" s="28"/>
       <c r="O236" s="50"/>
     </row>
-    <row r="237" spans="1:15">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A237" s="40" t="s">
         <v>1</v>
       </c>
@@ -5123,116 +5123,116 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.375" defaultRowHeight="14.1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="50.33203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="20" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="49" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="49" t="s">
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="49" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="49" t="s">
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="49" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="49" t="s">
+      <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="49" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="49" t="s">
+      <c r="B5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" s="49" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="49" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" s="49" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="49" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="49" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="49" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="49" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="49" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" s="49" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="49" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" s="49" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="49" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" s="49" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="49" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A13" s="49" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="49" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A14" s="49" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="49" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A15" s="49" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="49" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A16" s="49" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="49" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17" s="49" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="49" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A18" s="49" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="49" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19" s="49" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="49" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>